<commit_message>
actualizaciones recurso 60 y 80 tema 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC130.xlsx
+++ b/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC130.xlsx
@@ -546,9 +546,6 @@
     <t>Representar graficamente una funcion como la de la figura,  f(x)=-x^4+4</t>
   </si>
   <si>
-    <t>Una funcion como la que se muestra en la figura,  es necesario que al reflejarse en el eje x se obtenga la misma grafica y que tenga asintotas en -2 y 2</t>
-  </si>
-  <si>
     <t>Grafica de f(x)=cot(x-pi/2)</t>
   </si>
   <si>
@@ -583,6 +580,9 @@
   </si>
   <si>
     <t>MA_11_02_REC130</t>
+  </si>
+  <si>
+    <t>Una funcion como la que se muestra en la figura,  es necesario que al reflejarse en el eje y se obtenga la misma grafica y que tenga asintotas en -2 y 2</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,6 +784,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1300,7 +1306,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1473,16 +1479,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1568,6 +1566,26 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2809,9 +2827,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2849,14 +2867,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="F2" s="71" t="s">
+      <c r="D2" s="75"/>
+      <c r="F2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="72"/>
+      <c r="G2" s="68"/>
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
       <c r="J2" s="16"/>
@@ -2866,12 +2884,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="76">
         <v>11</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74"/>
+      <c r="D3" s="77"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="42"/>
       <c r="I3" s="42"/>
       <c r="J3" s="16"/>
@@ -2881,10 +2899,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="81"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="5"/>
       <c r="F4" s="41" t="s">
         <v>55</v>
@@ -2902,10 +2920,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="5"/>
       <c r="F5" s="39" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2938,7 +2956,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>39</v>
@@ -2956,12 +2974,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="77"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="73"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2998,7 +3016,7 @@
       <c r="I9" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="66" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="21" t="s">
@@ -3006,385 +3024,385 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="22" t="str">
+      <c r="C10" s="100" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F10" s="101" t="str">
         <f t="shared" ref="F10" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC130_IMG01n.png</v>
       </c>
-      <c r="G10" s="14" t="str">
+      <c r="G10" s="101" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H10" s="14" t="str">
+      <c r="H10" s="101" t="str">
         <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC130_IMG01a.png</v>
       </c>
-      <c r="I10" s="14" t="str">
+      <c r="I10" s="101" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="102"/>
+      <c r="K10" s="103" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="98" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="22" t="str">
+      <c r="C11" s="100" t="str">
         <f t="shared" ref="C11:C15" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="14" t="str">
+      <c r="F11" s="101" t="str">
         <f t="shared" ref="F11:F15" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC130_IMG02n.png</v>
       </c>
-      <c r="G11" s="14" t="str">
+      <c r="G11" s="101" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H11" s="14" t="str">
+      <c r="H11" s="101" t="str">
         <f t="shared" ref="H11:H15" si="3">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC130_IMG02a.png</v>
       </c>
-      <c r="I11" s="14" t="str">
+      <c r="I11" s="101" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="70" t="s">
+      <c r="J11" s="102"/>
+      <c r="K11" s="103" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="22" t="str">
+      <c r="C12" s="100" t="str">
         <f t="shared" si="1"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="14" t="str">
+      <c r="F12" s="101" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC130_IMG03n.png</v>
       </c>
-      <c r="G12" s="14" t="str">
+      <c r="G12" s="101" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H12" s="14" t="str">
+      <c r="H12" s="101" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC130_IMG03a.png</v>
       </c>
-      <c r="I12" s="14" t="str">
+      <c r="I12" s="101" t="str">
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="15" t="s">
-        <v>157</v>
+      <c r="J12" s="102"/>
+      <c r="K12" s="104" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="22" t="str">
+      <c r="C13" s="100" t="str">
         <f t="shared" si="1"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="14" t="str">
+      <c r="F13" s="101" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC130_IMG04n.png</v>
       </c>
-      <c r="G13" s="14" t="str">
+      <c r="G13" s="101" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H13" s="14" t="str">
+      <c r="H13" s="101" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC130_IMG04a.png</v>
       </c>
-      <c r="I13" s="14" t="str">
+      <c r="I13" s="101" t="str">
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J13" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="K13" s="66" t="s">
-        <v>158</v>
+      <c r="J13" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" s="105" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="22" t="str">
+      <c r="C14" s="100" t="str">
         <f t="shared" si="1"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="14" t="str">
+      <c r="F14" s="101" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC130_IMG05n.png</v>
       </c>
-      <c r="G14" s="14" t="str">
+      <c r="G14" s="101" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H14" s="14" t="str">
+      <c r="H14" s="101" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC130_IMG05a.png</v>
       </c>
-      <c r="I14" s="14" t="str">
+      <c r="I14" s="101" t="str">
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15" t="s">
-        <v>159</v>
+      <c r="J14" s="101"/>
+      <c r="K14" s="104" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="22" t="str">
+      <c r="C15" s="100" t="str">
         <f t="shared" si="1"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="101" t="str">
         <f t="shared" si="2"/>
         <v>MA_11_02_REC130_IMG06n.png</v>
       </c>
-      <c r="G15" s="14" t="str">
+      <c r="G15" s="101" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H15" s="14" t="str">
+      <c r="H15" s="101" t="str">
         <f t="shared" si="3"/>
         <v>MA_11_02_REC130_IMG06a.png</v>
       </c>
-      <c r="I15" s="14" t="str">
+      <c r="I15" s="101" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="66" t="s">
-        <v>160</v>
+      <c r="J15" s="101"/>
+      <c r="K15" s="105" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="68" t="s">
+      <c r="A16" s="98" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="22" t="str">
+      <c r="C16" s="100" t="str">
         <f t="shared" ref="C16:C18" si="4">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="14" t="str">
+      <c r="F16" s="101" t="str">
         <f t="shared" ref="F16:F18" si="5">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I16="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC130_IMG07n.png</v>
       </c>
-      <c r="G16" s="14" t="str">
+      <c r="G16" s="101" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H16" s="14" t="str">
+      <c r="H16" s="101" t="str">
         <f t="shared" ref="H16:H18" si="6">IF(AND(I16&lt;&gt;"",I16&lt;&gt;0),IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC130_IMG07a.png</v>
       </c>
-      <c r="I16" s="14" t="str">
+      <c r="I16" s="101" t="str">
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15" t="s">
-        <v>161</v>
+      <c r="J16" s="101"/>
+      <c r="K16" s="104" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="68" t="s">
+      <c r="A17" s="98" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="22" t="str">
+      <c r="C17" s="100" t="str">
         <f t="shared" si="4"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="14" t="str">
+      <c r="F17" s="101" t="str">
         <f t="shared" si="5"/>
         <v>MA_11_02_REC130_IMG08n.png</v>
       </c>
-      <c r="G17" s="14" t="str">
+      <c r="G17" s="101" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H17" s="14" t="str">
+      <c r="H17" s="101" t="str">
         <f t="shared" si="6"/>
         <v>MA_11_02_REC130_IMG08a.png</v>
       </c>
-      <c r="I17" s="14" t="str">
+      <c r="I17" s="101" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15" t="s">
-        <v>162</v>
+      <c r="J17" s="101"/>
+      <c r="K17" s="104" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="68" t="s">
+      <c r="A18" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="22" t="str">
+      <c r="C18" s="100" t="str">
         <f t="shared" si="4"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="14" t="str">
+      <c r="F18" s="101" t="str">
         <f t="shared" si="5"/>
         <v>MA_11_02_REC130_IMG09n.png</v>
       </c>
-      <c r="G18" s="14" t="str">
+      <c r="G18" s="101" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H18" s="14" t="str">
+      <c r="H18" s="101" t="str">
         <f t="shared" si="6"/>
         <v>MA_11_02_REC130_IMG09a.png</v>
       </c>
-      <c r="I18" s="14" t="str">
+      <c r="I18" s="101" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15" t="s">
+      <c r="J18" s="101"/>
+      <c r="K18" s="104" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="22" t="str">
+      <c r="C19" s="100" t="str">
         <f t="shared" ref="C19" si="7">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F19" s="14" t="str">
+      <c r="F19" s="101" t="str">
         <f t="shared" ref="F19" si="8">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC130_IMG10n.png</v>
       </c>
-      <c r="G19" s="14" t="str">
+      <c r="G19" s="101" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H19" s="14" t="str">
+      <c r="H19" s="101" t="str">
         <f t="shared" ref="H19" si="9">IF(AND(I19&lt;&gt;"",I19&lt;&gt;0),IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC130_IMG10a.png</v>
       </c>
-      <c r="I19" s="14" t="str">
+      <c r="I19" s="101" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="15" t="s">
-        <v>168</v>
+      <c r="J19" s="101"/>
+      <c r="K19" s="104" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4223,25 +4241,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="33"/>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -4249,11 +4267,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="97"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="34"/>
       <c r="H3" s="24" t="s">
         <v>18</v>
@@ -4304,11 +4322,11 @@
       <c r="C5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="98" t="str">
+      <c r="D5" s="94" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_02_CO</v>
       </c>
-      <c r="E5" s="99"/>
+      <c r="E5" s="95"/>
       <c r="F5" s="34"/>
       <c r="H5" s="24" t="s">
         <v>22</v>
@@ -4353,12 +4371,12 @@
       <c r="C7" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="84" t="str">
+      <c r="D7" s="80" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_CO.xls</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="85"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="81"/>
       <c r="H7" s="24" t="s">
         <v>24</v>
       </c>
@@ -4452,14 +4470,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84"/>
       <c r="I13" s="24" t="s">
         <v>33</v>
       </c>
@@ -4492,12 +4510,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="33"/>
-      <c r="C15" s="89" t="s">
+      <c r="C15" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="87"/>
       <c r="J15" s="24">
         <v>12</v>
       </c>
@@ -4537,12 +4555,12 @@
       <c r="C17" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="92" t="str">
+      <c r="D17" s="88" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_02_REC130</v>
       </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="90"/>
       <c r="J17" s="24">
         <v>14</v>
       </c>
@@ -4558,12 +4576,12 @@
       <c r="C18" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="84" t="str">
+      <c r="D18" s="80" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_REC130.xls</v>
       </c>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="81"/>
       <c r="J18" s="24">
         <v>15</v>
       </c>
@@ -4955,41 +4973,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="101" t="s">
+      <c r="H1" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="43" t="s">
         <v>65</v>
       </c>

</xml_diff>